<commit_message>
Updated Acceptance Criteria in Acceptance Test Plan
</commit_message>
<xml_diff>
--- a/etc/2225-swen-261-06-h-quackers.xlsx
+++ b/etc/2225-swen-261-06-h-quackers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mason Bausenwein\Desktop\School\2023 Spring Semester\SWEN-261\team-project-2225-swen-261-06-h-quackers\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DADB51-9220-4392-9695-0A1E8720DDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E693622A-EF5C-46F0-A2CD-63904B8E216C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="101">
   <si>
     <t>Instructions</t>
   </si>
@@ -63,12 +63,6 @@
 Submit this file per the instructions specified for the sprint submissions and cross-team testing.</t>
   </si>
   <si>
-    <t>As a Customer/Owner, I want to be able to view this page first and log in before being sent to my shopping cart and the catalog OR accessing admin tools depending on privileges.</t>
-  </si>
-  <si>
-    <t>**Given** I am in a browser **when** I submit a GET request to http://localhost:8080/login **then** I expect to see the log in page.</t>
-  </si>
-  <si>
     <t>**Given** I press the submit button **when** I have an admins login information in the input boxes **then** I expect to be redirected to the inventory management dashboard</t>
   </si>
   <si>
@@ -93,27 +87,12 @@
     <t>**Given** I AM LOGGED IN **when** I LOG OUT **then** I EXPECT MY DATA TO  NO LONGER PERSIST</t>
   </si>
   <si>
-    <t>**Given** I HAVE AN ACCOUNT **when** I LOG IN **then** MY DATA SHOULD APPEAR ON SCREEN</t>
-  </si>
-  <si>
     <t>As an owner I want to create be able to create a product so that my customers are able to buy it.</t>
   </si>
   <si>
-    <t>**Given** I am an owner **when** I go to the product creation page (http://localhost:4200/inventory/product) **then** I expect to see a form that I can fill out that allows me to input all of the necessary information (i.e. name, size, etc -- NOT ID)</t>
-  </si>
-  <si>
-    <t>**Given** I am a buyer **when** I go to the product creation page (http://localhost:4200/inventory/product) **then** I expect to see an error pop up and be redirected to the login page.</t>
-  </si>
-  <si>
     <t>As an OWNER I want to be able to modify products so that I can change the price, quantity available, name, etc of my items.</t>
   </si>
   <si>
-    <t>**Given** I am a buyer **when** I go to the inventory management page (http://localhost:4200/inventory/product/{id}) **then** I expect to see an error pop up and be redirected to the login page.</t>
-  </si>
-  <si>
-    <t>**Given** I am an owner **when** I hit the submit button on a product management page (http://localhost:4200/inventory/product/{id}) **then** I expect to see a success message.</t>
-  </si>
-  <si>
     <t>As an OWNER I want to SEE PRODUCTS ON THE INVENTORY MANAGEMENT PAGE so that I CAN SELECT THEM TO MODIFY.</t>
   </si>
   <si>
@@ -144,12 +123,6 @@
     <t>As a BUYER I want to HAVE A PROFILE PAGE so that I CAN SAVE MY PAYMENT AND SHIPPING INFORMATION.</t>
   </si>
   <si>
-    <t>**Given** I am an owner or not logged in **when** I attempt to access my profile page **then** I expect to be redirected to the login screen and see an error</t>
-  </si>
-  <si>
-    <t>**Given** I am a buyer **when** I attempt to access my profile page **then** I expect to see a screen where I can save my payment and shipping information along with a save button and a clear button</t>
-  </si>
-  <si>
     <t>As a CUSTOMER I want to SEE A RECEIPT OF THE ITEMS I PURCHASED so that I CAN MAKE SURE I BOUGHT EVERYTHING I WANT</t>
   </si>
   <si>
@@ -171,9 +144,6 @@
     <t>**Given** I am an owner **when** I click the remove button **then** I expect the product to be deleted and to see a success notification if successful or an error notification if not</t>
   </si>
   <si>
-    <t>**Given** I am an owner **when** I go to the product management page (http://localhost:4200/inventory/product/{id}) **then** I expect to see all of the fields I can modify and a save button</t>
-  </si>
-  <si>
     <t>As an BUYER I want to SEE PRODUCTS ON THE CATALOG PAGE so that I ADD THEM MY SHOPPING CART.</t>
   </si>
   <si>
@@ -225,18 +195,9 @@
     <t>Mason Bausenwein; March 18th</t>
   </si>
   <si>
-    <t>**Given** I am logged in as a buyer and I am on a browser **when** I click the shopping cart button or submit a get request to http://localhost:8080/cart **then** I expect to see my shopping cart (items - name, price, quantity in cart, cart - price total).</t>
-  </si>
-  <si>
-    <t>**Given** I am logged in as a owner or not logged in **when** I go to http://localhost:8080/cart **then** I expect to see an error pop up and be redirected to the login page</t>
-  </si>
-  <si>
     <t>**Given** I am logged in as a buyer **when** I click the remove button **then** I expect the correct amount of the item corresponding to the remove button to be removed</t>
   </si>
   <si>
-    <t>**Given** I am logged in as a buyer **when** I click the back button **then** I expect to be directed back to https://localhost:8080/catalog or http://localhost:8080/catalog/:id (use location.back -- need to inject Location in the constructor)</t>
-  </si>
-  <si>
     <t>**Given** I am logged in as a buyer and have items in my cart **when** I click the clear cart button **then** I expect my cart to be cleared</t>
   </si>
   <si>
@@ -273,18 +234,9 @@
     <t>As an OWNER I want the catalog/inventory management pages to look nice and be easy to use so that I and my customers do not get confused and have a nice experience.</t>
   </si>
   <si>
-    <t>**Given** I am logged in as a buyer **when** I go to the catalog page **then** I expect to see all of the items listed in boxes with drop shadows. (The boxes should contain the following: name of the duck, price of the duck, and quantity available. There should also be a selector that allows them to add as many ducks to the cart as they like and a view item button)</t>
-  </si>
-  <si>
-    <t>**Given** I am logged in as a buyer **when** I am on the catalog page **then** I expect to see a go-to cart button (use angular material buttons)</t>
-  </si>
-  <si>
     <t>**Given** I am logged in as an owner **when** I go to the inventory management page **then** I expect to see all of the items listed in boxes with drop shadows. (The boxes should contain the following: name of the duck, price of the duck, and quantity available. There should also be a modify button and a remove button)</t>
   </si>
   <si>
-    <t>**Given** I am on the inventory management page **when** I click the modify item button on an item **then** I expect to be taken to the modify product page (make this a modal)</t>
-  </si>
-  <si>
     <t>**Given** I am logged in **when** I am on the catalog/inventory management page **then** I expect all of the items to have pictures that reflect their outfit/color/size properties</t>
   </si>
   <si>
@@ -321,9 +273,6 @@
     <t>As a BUYER I want to HAVE A CUSTOMIZABLE DUCK PAGE so that I CAN CUSTOMIZE MY OWN DUCK AND ADD IT TO MY SHOPPING CART.</t>
   </si>
   <si>
-    <t>**Given** I am a buyer **when** I attempt to access the customize page **then** I expect to see a screen where I can customize my own duck along with a button to add to my cart</t>
-  </si>
-  <si>
     <t>**Given** I am a buyer **when** create my own duck **then** I expect to customize features of my duck such as its name, size, color, and outfit which includes its hat, hand item, and jewelry.</t>
   </si>
   <si>
@@ -331,6 +280,60 @@
   </si>
   <si>
     <t>Mason Bausenwein; April 3rd; This acceptance criteria was not defined during sprint 2, but is being marked as failing for completion of this document</t>
+  </si>
+  <si>
+    <t>As a Customer/Owner, I want to be able to view the login page first and log in before being sent to my shopping cart and the catalog OR accessing admin tools depending on privileges.</t>
+  </si>
+  <si>
+    <t>**Given** I am in a browser **when** I submit a go to the website **then** I expect to see the log in page.</t>
+  </si>
+  <si>
+    <t>**Given** I am an owner **when** I hit the submit button on a product management page  **then** I expect to see a success message.</t>
+  </si>
+  <si>
+    <t>**Given** I am a buyer **when** I go to the inventory management page  **then** I expect to see an error pop up and be redirected to the login page.</t>
+  </si>
+  <si>
+    <t>**Given** I am an owner **when** I go to the product management page  **then** I expect to see all of the fields I can modify and a save button</t>
+  </si>
+  <si>
+    <t>**Given** I am logged in as a buyer and I am on a browser **when** I click the shopping cart button **then** I expect to see my shopping cart (items - name, price, quantity in cart, cart - price total).</t>
+  </si>
+  <si>
+    <t>**Given** I am logged in as an owner or not logged in **when** I go to the cart page **then** I expect to see an error pop up and be redirected to the login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Given** I am logged in as a buyer **when** I click the back button **then** I expect to be directed back to the previous page I was on </t>
+  </si>
+  <si>
+    <t>Mason Bausenwein; April 4th. The product view page was removed because it was deemed no longer necessary after the duck images were implemented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mason Bausenwein; April 4th. In Sprint 3, a quantity input was added in place of the view detail to allow for a variable number of ducks to be added to cart from the catalog page </t>
+  </si>
+  <si>
+    <t>**Given** I am logged in as a buyer **when** I go to the catalog page **then** I expect to see all of the items listed in boxes with drop shadows. (The boxes should contain the following: name of the duck, price of the duck, and quantity available. There should also be a selector that allows them to add as many ducks to the cart as they like)</t>
+  </si>
+  <si>
+    <t>**Given** I am on the inventory management page **when** I click the modify item button on an item **then** I expect the modify product modal to open</t>
+  </si>
+  <si>
+    <t>**Given** I am logged in as a buyer **when** I am on the catalog page **then** I expect to see a go-to cart button</t>
+  </si>
+  <si>
+    <t>**Given** I HAVE AN ACCOUNT **when** I LOG IN **then** MY ACCOUNT SHOULD BE STORED (i.e. shopping cart should be loaded)</t>
+  </si>
+  <si>
+    <t>**Given** I am an owner **when** I go to the product creation page **then** I expect to see a form that I can fill out that allows me to input all of the necessary information (i.e. name, size, etc -- NOT ID)</t>
+  </si>
+  <si>
+    <t>**Given** I am a buyer **when** I go to the product creation page  **then** I expect to see an error pop up and be redirected to the login page.</t>
+  </si>
+  <si>
+    <t>Mason Bausenwein; April 4th. This is no longer a page but rather a modal</t>
+  </si>
+  <si>
+    <t>**Given** I am a buyer **when** I attempt to access the customize modal **then** I expect to see a screen where I can customize my own duck along with a button to add to my cart</t>
   </si>
 </sst>
 </file>
@@ -839,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -862,11 +865,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F607"/>
+  <dimension ref="A1:F610"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -902,870 +905,914 @@
     </row>
     <row r="2" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E11" s="7"/>
+      <c r="F11" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E12" s="7"/>
+      <c r="F12" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E13" s="7"/>
+      <c r="F13" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E15" s="7"/>
+      <c r="F15" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="10" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="10" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="F31" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C32" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="F32" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="10" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="F38" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
       <c r="B41" s="10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>41</v>
-      </c>
+    <row r="43" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="7"/>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>36</v>
-      </c>
+    <row r="44" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C44" s="7"/>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>99</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C45" s="7"/>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>92</v>
+    <row r="46" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B47" s="2" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10" t="s">
-        <v>94</v>
+    <row r="48" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="49" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="10"/>
       <c r="B51" s="10" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10"/>
       <c r="B54" s="10" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
+    <row r="57" spans="1:5" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="B58" s="2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E58" s="7"/>
     </row>
     <row r="59" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10" t="s">
-        <v>85</v>
+    <row r="60" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="B61" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10"/>
       <c r="B63" s="10" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="10"/>
       <c r="B66" s="10" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C67" s="7"/>
+    <row r="67" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C68" s="7"/>
+    <row r="68" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C69" s="7"/>
+    <row r="69" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="10"/>
+      <c r="B69" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="E69" s="7"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3920,9 +3967,21 @@
       <c r="C607" s="7"/>
       <c r="E607" s="7"/>
     </row>
+    <row r="608" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C608" s="7"/>
+      <c r="E608" s="7"/>
+    </row>
+    <row r="609" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C609" s="7"/>
+      <c r="E609" s="7"/>
+    </row>
+    <row r="610" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C610" s="7"/>
+      <c r="E610" s="7"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E607 C2:C607">
+  <conditionalFormatting sqref="E2:E610 C2:C610">
     <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -3930,7 +3989,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F607 D2:D607">
+  <conditionalFormatting sqref="D2:D610 F2:F610">
     <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
@@ -3939,7 +3998,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31 E2:E607 C33:C607" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31 E2:E610 C33:C610" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fixed minor bugs and updated acceptance test plan
</commit_message>
<xml_diff>
--- a/etc/2225-swen-261-06-h-quackers.xlsx
+++ b/etc/2225-swen-261-06-h-quackers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mason Bausenwein\Desktop\School\2023 Spring Semester\SWEN-261\team-project-2225-swen-261-06-h-quackers\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E693622A-EF5C-46F0-A2CD-63904B8E216C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F270C0D5-714A-42A2-82DA-506F1E0C95E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22670" yWindow="-740" windowWidth="22780" windowHeight="14540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="108">
   <si>
     <t>Instructions</t>
   </si>
@@ -66,12 +66,6 @@
     <t>**Given** I press the submit button **when** I have an admins login information in the input boxes **then** I expect to be redirected to the inventory management dashboard</t>
   </si>
   <si>
-    <t>**Given** I press the submit button **when** I have anything that is not admin entered in the username box **then** I expect to be redirected to the product view dashboard</t>
-  </si>
-  <si>
-    <t>**Given **I press the submit button **when** account information is entered **then** I expect the account information to stay in the session (basically, have account information present on the page)</t>
-  </si>
-  <si>
     <t>**Given **I press the register button **when **account information is entered and doesn't exist already, **then **I expect the account to be registered to the database and have a feedback message appear saying account was created.</t>
   </si>
   <si>
@@ -255,9 +249,6 @@
     <t>**Given** I click the reset password button **when** I have entered a username for an nonexistant account **then** I expect to receive an error snackbar saying account does not exist</t>
   </si>
   <si>
-    <t>**Given** I am a buyer **when** I attempt to access my profile page **then** I expect to see a screen where I can save my payment and shipping information along with a save button</t>
-  </si>
-  <si>
     <t>**Given** I am on the profile page **when** I attempt to click the change payment information button **then** I expect to see a screen where I can modify my payment information</t>
   </si>
   <si>
@@ -321,19 +312,49 @@
     <t>**Given** I am logged in as a buyer **when** I am on the catalog page **then** I expect to see a go-to cart button</t>
   </si>
   <si>
-    <t>**Given** I HAVE AN ACCOUNT **when** I LOG IN **then** MY ACCOUNT SHOULD BE STORED (i.e. shopping cart should be loaded)</t>
-  </si>
-  <si>
     <t>**Given** I am an owner **when** I go to the product creation page **then** I expect to see a form that I can fill out that allows me to input all of the necessary information (i.e. name, size, etc -- NOT ID)</t>
   </si>
   <si>
-    <t>**Given** I am a buyer **when** I go to the product creation page  **then** I expect to see an error pop up and be redirected to the login page.</t>
-  </si>
-  <si>
-    <t>Mason Bausenwein; April 4th. This is no longer a page but rather a modal</t>
-  </si>
-  <si>
     <t>**Given** I am a buyer **when** I attempt to access the customize modal **then** I expect to see a screen where I can customize my own duck along with a button to add to my cart</t>
+  </si>
+  <si>
+    <t>**Given** I press the submit button **when** I am logging in with a valid account that does not have the username admin **then** I expect to be redirected to the product view dashboard</t>
+  </si>
+  <si>
+    <t>**Given **I press the submit button **when** account information is entered **then** I expect the account information to stay in the session (basically, I stay logged in when switching pages)</t>
+  </si>
+  <si>
+    <t>Mason Bausenwein; April 4th</t>
+  </si>
+  <si>
+    <t>Mason Bausenwein; April 4th; Password must be considered strong</t>
+  </si>
+  <si>
+    <t>**Given** I HAVE AN ACCOUNT **when** I LOG IN **then** MY ACCOUNT SHOULD BE STORED (i.e. shopping cart page should show my cart)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Given** I am a buyer **when** I go to the product creation page  **then** I expect to see an error pop up and be redirected to the login page. </t>
+  </si>
+  <si>
+    <t>Mason Bausenwein; April 4th; Not even possible for buyers to even access this page anymore because it is a modal</t>
+  </si>
+  <si>
+    <t>Mason Bausenwein; April 4th; This is no longer a page but rather a modal</t>
+  </si>
+  <si>
+    <t>Mason Bausenwein; April 4th; There is now a quantity selector so multiple items can be added rather than just one. However, 1 is the default value</t>
+  </si>
+  <si>
+    <t>Mason Bausenwein; April 4th; Search is case sensitive</t>
+  </si>
+  <si>
+    <t>**Given** I am a buyer **when** I attempt to access my profile page **then** I expect to see a screen where I can change my payment and shipping information along with a close button</t>
+  </si>
+  <si>
+    <t>Mason Bausenwein; April 4th; Realistically, it is not possible for this to actually occur due to prior validation when the shopping cart page loads. However, it does work</t>
+  </si>
+  <si>
+    <t>Mason Bausenwein; April 4th; This is now a modal and not a page</t>
   </si>
 </sst>
 </file>
@@ -370,12 +391,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -408,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -436,6 +463,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -842,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -865,11 +895,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F610"/>
+  <dimension ref="A1:F605"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B60" sqref="B60"/>
+      <selection pane="topRight" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -905,18 +935,23 @@
     </row>
     <row r="2" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
@@ -924,938 +959,1169 @@
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F11" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F13" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F14" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>91</v>
+        <v>29</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>91</v>
+        <v>29</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E36" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E38" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>91</v>
+        <v>29</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E39" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
       <c r="B41" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E42" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="E43" s="7"/>
+      <c r="E43" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="E44" s="7"/>
+      <c r="E44" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="E45" s="7"/>
+      <c r="E45" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10"/>
       <c r="B46" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
+      <c r="B52" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="10"/>
+      <c r="B61" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
+      <c r="B64" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="C64" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E49" s="7"/>
-    </row>
-    <row r="50" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="7"/>
-    </row>
-    <row r="51" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E51" s="7"/>
-    </row>
-    <row r="52" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" s="7"/>
-    </row>
-    <row r="53" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E53" s="7"/>
-    </row>
-    <row r="54" spans="1:5" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E54" s="7"/>
-    </row>
-    <row r="55" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E55" s="7"/>
-    </row>
-    <row r="56" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E56" s="7"/>
-    </row>
-    <row r="57" spans="1:5" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E57" s="7"/>
-    </row>
-    <row r="58" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E58" s="7"/>
-    </row>
-    <row r="59" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E59" s="7"/>
-    </row>
-    <row r="60" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E60" s="7"/>
-    </row>
-    <row r="61" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E61" s="7"/>
-    </row>
-    <row r="62" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B62" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62" s="7"/>
-    </row>
-    <row r="63" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E63" s="7"/>
-    </row>
-    <row r="64" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="D64" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E64" s="7"/>
-    </row>
-    <row r="65" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65" s="7"/>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="10"/>
-      <c r="B66" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>82</v>
-      </c>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C66" s="7"/>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>82</v>
-      </c>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C67" s="7"/>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B68" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>82</v>
-      </c>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C68" s="7"/>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>82</v>
-      </c>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C69" s="7"/>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C70" s="7"/>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C71" s="7"/>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C72" s="7"/>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C73" s="7"/>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C74" s="7"/>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C75" s="7"/>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C77" s="7"/>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C78" s="7"/>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C79" s="7"/>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C80" s="7"/>
       <c r="E80" s="7"/>
     </row>
@@ -3959,29 +4225,9 @@
       <c r="C605" s="7"/>
       <c r="E605" s="7"/>
     </row>
-    <row r="606" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C606" s="7"/>
-      <c r="E606" s="7"/>
-    </row>
-    <row r="607" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C607" s="7"/>
-      <c r="E607" s="7"/>
-    </row>
-    <row r="608" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C608" s="7"/>
-      <c r="E608" s="7"/>
-    </row>
-    <row r="609" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C609" s="7"/>
-      <c r="E609" s="7"/>
-    </row>
-    <row r="610" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C610" s="7"/>
-      <c r="E610" s="7"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E610 C2:C610">
+  <conditionalFormatting sqref="C2:C605 E2:E605">
     <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -3989,7 +4235,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D610 F2:F610">
+  <conditionalFormatting sqref="D2:D605 F2:F605">
     <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
@@ -3998,7 +4244,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31 E2:E610 C33:C610" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31 E2:E605 C33:C605" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>